<commit_message>
Autolvler AI Agent deepening KnowledgeBase
</commit_message>
<xml_diff>
--- a/Accountant.xlsx
+++ b/Accountant.xlsx
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>569</v>
+        <v>662</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>569</v>
+        <v>662</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
AI Agent probability distribution work
</commit_message>
<xml_diff>
--- a/Accountant.xlsx
+++ b/Accountant.xlsx
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>662</v>
+        <v>932</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>662</v>
+        <v>932</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
AI Agent lvler work
</commit_message>
<xml_diff>
--- a/Accountant.xlsx
+++ b/Accountant.xlsx
@@ -460,7 +460,7 @@
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="9" customWidth="1" min="7" max="7"/>
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>932</v>
+        <v>1580</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>932</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="3">
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved_stuck logic, expanding stuck AI knowledge base
</commit_message>
<xml_diff>
--- a/Accountant.xlsx
+++ b/Accountant.xlsx
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1580</v>
+        <v>1758</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1580</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="3">
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improving timings & AI reading the state of the world regarding stuck()
</commit_message>
<xml_diff>
--- a/Accountant.xlsx
+++ b/Accountant.xlsx
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1758</v>
+        <v>1835</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1758</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="3">
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AI agent further expanding knowledge base
</commit_message>
<xml_diff>
--- a/Accountant.xlsx
+++ b/Accountant.xlsx
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1835</v>
+        <v>2060</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1835</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="3">
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refining timings & blueprints
</commit_message>
<xml_diff>
--- a/Accountant.xlsx
+++ b/Accountant.xlsx
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>2060</v>
+        <v>2290</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>2060</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="3">
@@ -537,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -546,7 +546,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>